<commit_message>
updated learn list xls files
</commit_message>
<xml_diff>
--- a/lists/learn_list_study4_c3.xlsx
+++ b/lists/learn_list_study4_c3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gelliott/Documents/projects/delaylearn/feedback-delay-four/lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D240A8AA-6E8E-8D49-B6C0-39204EE229F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACA38E1-3308-9345-BB58-53BCFA42F35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3740" yWindow="500" windowWidth="43380" windowHeight="27560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -698,7 +698,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -711,6 +711,12 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1068,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E25E4B-9AFA-2443-8C1F-D7B80241CF51}">
   <dimension ref="A1:AB115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1:Z115"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8:I115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1085,7 +1091,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B1" t="s">
@@ -1148,7 +1154,7 @@
       <c r="U1" t="s">
         <v>42</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="6" t="s">
         <v>33</v>
       </c>
       <c r="W1" s="1" t="s">
@@ -1165,7 +1171,7 @@
       </c>
     </row>
     <row r="2" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2">
@@ -1228,7 +1234,7 @@
       <c r="U2" t="s">
         <v>51</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="5">
         <v>1</v>
       </c>
       <c r="W2" t="s">
@@ -1245,7 +1251,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3">
@@ -1308,7 +1314,7 @@
       <c r="U3" t="s">
         <v>51</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="5">
         <v>1</v>
       </c>
       <c r="W3" t="s">
@@ -1325,7 +1331,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4">
@@ -1388,7 +1394,7 @@
       <c r="U4" t="s">
         <v>51</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="5">
         <v>0</v>
       </c>
       <c r="W4" t="s">
@@ -1405,7 +1411,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5">
@@ -1468,7 +1474,7 @@
       <c r="U5" t="s">
         <v>51</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="5">
         <v>1</v>
       </c>
       <c r="W5" t="s">
@@ -1485,7 +1491,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6">
@@ -1548,7 +1554,7 @@
       <c r="U6" t="s">
         <v>51</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="5">
         <v>1</v>
       </c>
       <c r="W6" t="s">
@@ -1565,7 +1571,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7">
@@ -1628,7 +1634,7 @@
       <c r="U7" t="s">
         <v>51</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="5">
         <v>1</v>
       </c>
       <c r="W7" t="s">
@@ -1645,7 +1651,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8">
@@ -1674,7 +1680,7 @@
         <v>57</v>
       </c>
       <c r="I8" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="J8">
         <v>7000</v>
@@ -1716,7 +1722,7 @@
         <f t="shared" ref="U8:U39" si="7">CONCATENATE("images/choice_trial_",Q8,".png")</f>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V8">
+      <c r="V8" s="5">
         <v>1</v>
       </c>
       <c r="W8" t="s">
@@ -1734,7 +1740,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9">
@@ -1763,7 +1769,7 @@
         <v>57</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="J9">
         <v>750</v>
@@ -1805,7 +1811,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="5">
         <v>1</v>
       </c>
       <c r="W9" t="s">
@@ -1823,7 +1829,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10">
@@ -1852,7 +1858,7 @@
         <v>57</v>
       </c>
       <c r="I10" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J10">
         <v>7000</v>
@@ -1894,7 +1900,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="5">
         <v>1</v>
       </c>
       <c r="W10" t="s">
@@ -1912,7 +1918,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11">
@@ -1941,7 +1947,7 @@
         <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="J11">
         <v>750</v>
@@ -1983,7 +1989,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="5">
         <v>1</v>
       </c>
       <c r="W11" t="s">
@@ -2001,22 +2007,22 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>images/choice_trial_13.png</v>
+        <v>images/choice_trial_14.png</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>images/choice_trial_10.png</v>
+        <v>images/choice_trial_8.png</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="2"/>
@@ -2030,19 +2036,19 @@
         <v>57</v>
       </c>
       <c r="I12" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="J12">
         <v>750</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N12">
         <v>6</v>
@@ -2051,28 +2057,28 @@
         <v>5</v>
       </c>
       <c r="P12" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Q12" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="R12">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S12">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T12" t="str">
         <f t="shared" si="6"/>
-        <v>images/choice_trial_13.png</v>
+        <v>images/choice_trial_14.png</v>
       </c>
       <c r="U12" t="str">
         <f t="shared" si="7"/>
-        <v>images/choice_trial_10.png</v>
-      </c>
-      <c r="V12">
+        <v>images/choice_trial_8.png</v>
+      </c>
+      <c r="V12" s="5">
         <v>0</v>
       </c>
       <c r="W12" t="s">
@@ -2090,7 +2096,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13">
@@ -2119,7 +2125,7 @@
         <v>57</v>
       </c>
       <c r="I13" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J13">
         <v>7000</v>
@@ -2161,7 +2167,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V13">
+      <c r="V13" s="5">
         <v>1</v>
       </c>
       <c r="W13" t="s">
@@ -2179,7 +2185,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14">
@@ -2208,7 +2214,7 @@
         <v>57</v>
       </c>
       <c r="I14" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="J14">
         <v>7000</v>
@@ -2250,7 +2256,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="5">
         <v>0</v>
       </c>
       <c r="W14" t="s">
@@ -2268,7 +2274,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15">
@@ -2297,7 +2303,7 @@
         <v>57</v>
       </c>
       <c r="I15" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="J15">
         <v>750</v>
@@ -2339,7 +2345,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V15">
+      <c r="V15" s="5">
         <v>1</v>
       </c>
       <c r="W15" t="s">
@@ -2357,22 +2363,22 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>images/choice_trial_14.png</v>
+        <v>images/choice_trial_13.png</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
-        <v>images/choice_trial_8.png</v>
+        <v>images/choice_trial_10.png</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="2"/>
@@ -2380,25 +2386,25 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="3"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="H16" t="s">
         <v>57</v>
       </c>
       <c r="I16" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="J16">
         <v>750</v>
       </c>
       <c r="K16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N16">
         <v>6</v>
@@ -2407,36 +2413,36 @@
         <v>5</v>
       </c>
       <c r="P16" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q16" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="R16">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S16">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="T16" t="str">
         <f t="shared" si="6"/>
-        <v>images/choice_trial_14.png</v>
+        <v>images/choice_trial_13.png</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" si="7"/>
-        <v>images/choice_trial_8.png</v>
-      </c>
-      <c r="V16">
-        <v>0</v>
+        <v>images/choice_trial_10.png</v>
+      </c>
+      <c r="V16" s="5">
+        <v>1</v>
       </c>
       <c r="W16" t="s">
         <v>8</v>
       </c>
       <c r="X16" t="str">
         <f t="shared" si="8"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="Y16">
         <v>0</v>
@@ -2446,7 +2452,7 @@
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17">
@@ -2475,7 +2481,7 @@
         <v>57</v>
       </c>
       <c r="I17" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J17">
         <v>7000</v>
@@ -2517,7 +2523,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V17">
+      <c r="V17" s="5">
         <v>1</v>
       </c>
       <c r="W17" t="s">
@@ -2535,7 +2541,7 @@
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18">
@@ -2558,13 +2564,13 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" si="3"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="H18" t="s">
         <v>57</v>
       </c>
       <c r="I18" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="J18">
         <v>750</v>
@@ -2606,15 +2612,15 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V18">
-        <v>1</v>
+      <c r="V18" s="5">
+        <v>0</v>
       </c>
       <c r="W18" t="s">
         <v>8</v>
       </c>
       <c r="X18" t="str">
         <f t="shared" si="8"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="Y18">
         <v>0</v>
@@ -2624,7 +2630,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19">
@@ -2653,7 +2659,7 @@
         <v>57</v>
       </c>
       <c r="I19" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J19">
         <v>7000</v>
@@ -2695,7 +2701,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V19">
+      <c r="V19" s="5">
         <v>1</v>
       </c>
       <c r="W19" t="s">
@@ -2713,7 +2719,7 @@
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
       <c r="B20">
@@ -2742,7 +2748,7 @@
         <v>57</v>
       </c>
       <c r="I20" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="J20">
         <v>750</v>
@@ -2784,7 +2790,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V20">
+      <c r="V20" s="5">
         <v>1</v>
       </c>
       <c r="W20" t="s">
@@ -2802,7 +2808,7 @@
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
       <c r="B21">
@@ -2831,7 +2837,7 @@
         <v>57</v>
       </c>
       <c r="I21" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J21">
         <v>7000</v>
@@ -2873,7 +2879,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V21">
+      <c r="V21" s="5">
         <v>1</v>
       </c>
       <c r="W21" t="s">
@@ -2891,7 +2897,7 @@
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
       <c r="B22">
@@ -2920,7 +2926,7 @@
         <v>57</v>
       </c>
       <c r="I22" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="J22">
         <v>750</v>
@@ -2962,7 +2968,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V22">
+      <c r="V22" s="5">
         <v>1</v>
       </c>
       <c r="W22" t="s">
@@ -2980,7 +2986,7 @@
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
       <c r="B23">
@@ -3003,13 +3009,13 @@
       </c>
       <c r="G23" t="str">
         <f t="shared" si="3"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="H23" t="s">
         <v>57</v>
       </c>
       <c r="I23" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="J23">
         <v>7000</v>
@@ -3051,15 +3057,15 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V23">
-        <v>1</v>
+      <c r="V23" s="5">
+        <v>0</v>
       </c>
       <c r="W23" t="s">
         <v>8</v>
       </c>
       <c r="X23" t="str">
         <f t="shared" si="8"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="Y23">
         <v>1</v>
@@ -3069,14 +3075,14 @@
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
@@ -3092,16 +3098,16 @@
       </c>
       <c r="G24" t="str">
         <f t="shared" si="3"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="H24" t="s">
         <v>57</v>
       </c>
       <c r="I24" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="J24">
-        <v>7000</v>
+        <v>750</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -3113,10 +3119,10 @@
         <v>3</v>
       </c>
       <c r="N24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P24" s="4">
         <v>15</v>
@@ -3140,32 +3146,32 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V24">
-        <v>0</v>
+      <c r="V24" s="5">
+        <v>1</v>
       </c>
       <c r="W24" t="s">
         <v>8</v>
       </c>
       <c r="X24" t="str">
         <f t="shared" si="8"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="Y24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="5">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
@@ -3187,10 +3193,10 @@
         <v>57</v>
       </c>
       <c r="I25" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="J25">
-        <v>750</v>
+        <v>7000</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -3202,10 +3208,10 @@
         <v>3</v>
       </c>
       <c r="N25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P25" s="4">
         <v>15</v>
@@ -3229,7 +3235,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V25">
+      <c r="V25" s="5">
         <v>1</v>
       </c>
       <c r="W25" t="s">
@@ -3240,14 +3246,14 @@
         <v>f</v>
       </c>
       <c r="Y25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
       <c r="B26">
@@ -3276,7 +3282,7 @@
         <v>57</v>
       </c>
       <c r="I26" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="J26">
         <v>750</v>
@@ -3318,7 +3324,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V26">
+      <c r="V26" s="5">
         <v>1</v>
       </c>
       <c r="W26" t="s">
@@ -3336,7 +3342,7 @@
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27">
@@ -3365,7 +3371,7 @@
         <v>57</v>
       </c>
       <c r="I27" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J27">
         <v>7000</v>
@@ -3407,7 +3413,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V27">
+      <c r="V27" s="5">
         <v>1</v>
       </c>
       <c r="W27" t="s">
@@ -3425,54 +3431,54 @@
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>images/choice_trial_2.png</v>
+        <v>images/choice_trial_11.png</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="1"/>
-        <v>images/choice_trial_11.png</v>
+        <v>images/choice_trial_2.png</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="2"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="3"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="H28" t="s">
         <v>57</v>
       </c>
       <c r="I28" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="J28">
         <v>750</v>
       </c>
       <c r="K28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28">
         <v>4</v>
       </c>
       <c r="N28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P28" s="4">
         <v>11</v>
@@ -3482,11 +3488,11 @@
       </c>
       <c r="R28">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="S28">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="T28" t="str">
         <f t="shared" si="6"/>
@@ -3496,7 +3502,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V28">
+      <c r="V28" s="5">
         <v>1</v>
       </c>
       <c r="W28" t="s">
@@ -3514,54 +3520,54 @@
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="5">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>images/choice_trial_11.png</v>
+        <v>images/choice_trial_2.png</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="1"/>
-        <v>images/choice_trial_2.png</v>
+        <v>images/choice_trial_11.png</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="2"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="3"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="H29" t="s">
         <v>57</v>
       </c>
       <c r="I29" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="J29">
         <v>750</v>
       </c>
       <c r="K29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29">
         <v>4</v>
       </c>
       <c r="N29">
+        <v>6</v>
+      </c>
+      <c r="O29">
         <v>5</v>
-      </c>
-      <c r="O29">
-        <v>4</v>
       </c>
       <c r="P29" s="4">
         <v>11</v>
@@ -3571,11 +3577,11 @@
       </c>
       <c r="R29">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="S29">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="T29" t="str">
         <f t="shared" si="6"/>
@@ -3585,7 +3591,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V29">
+      <c r="V29" s="5">
         <v>1</v>
       </c>
       <c r="W29" t="s">
@@ -3603,7 +3609,7 @@
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="5">
         <v>29</v>
       </c>
       <c r="B30">
@@ -3632,7 +3638,7 @@
         <v>57</v>
       </c>
       <c r="I30" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J30">
         <v>7000</v>
@@ -3674,7 +3680,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V30">
+      <c r="V30" s="5">
         <v>1</v>
       </c>
       <c r="W30" t="s">
@@ -3692,7 +3698,7 @@
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
       <c r="B31">
@@ -3721,7 +3727,7 @@
         <v>57</v>
       </c>
       <c r="I31" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="J31">
         <v>7000</v>
@@ -3763,7 +3769,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V31">
+      <c r="V31" s="5">
         <v>1</v>
       </c>
       <c r="W31" t="s">
@@ -3781,14 +3787,14 @@
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="5">
         <v>31</v>
       </c>
       <c r="B32">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
@@ -3804,19 +3810,19 @@
       </c>
       <c r="G32" t="str">
         <f t="shared" si="3"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="H32" t="s">
         <v>57</v>
       </c>
       <c r="I32" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J32">
-        <v>7000</v>
+        <v>750</v>
       </c>
       <c r="K32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -3825,15 +3831,15 @@
         <v>5</v>
       </c>
       <c r="N32">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="O32">
-        <v>1</v>
-      </c>
-      <c r="P32">
+        <v>4</v>
+      </c>
+      <c r="P32" s="4">
         <v>16</v>
       </c>
-      <c r="Q32">
+      <c r="Q32" s="4">
         <v>3</v>
       </c>
       <c r="R32">
@@ -3852,32 +3858,32 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V32">
-        <v>1</v>
+      <c r="V32" s="5">
+        <v>0</v>
       </c>
       <c r="W32" t="s">
         <v>8</v>
       </c>
       <c r="X32" t="str">
         <f t="shared" si="8"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="Y32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z32">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="5">
         <v>32</v>
       </c>
       <c r="B33">
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
@@ -3899,13 +3905,13 @@
         <v>57</v>
       </c>
       <c r="I33" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="J33">
-        <v>750</v>
+        <v>7000</v>
       </c>
       <c r="K33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L33">
         <v>0</v>
@@ -3914,15 +3920,15 @@
         <v>5</v>
       </c>
       <c r="N33">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="O33">
-        <v>5</v>
-      </c>
-      <c r="P33" s="4">
+        <v>1</v>
+      </c>
+      <c r="P33">
         <v>16</v>
       </c>
-      <c r="Q33" s="4">
+      <c r="Q33">
         <v>3</v>
       </c>
       <c r="R33">
@@ -3941,7 +3947,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V33">
+      <c r="V33" s="5">
         <v>1</v>
       </c>
       <c r="W33" t="s">
@@ -3952,21 +3958,21 @@
         <v>f</v>
       </c>
       <c r="Y33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z33">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" s="5">
         <v>33</v>
       </c>
       <c r="B34">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
@@ -3988,7 +3994,7 @@
         <v>57</v>
       </c>
       <c r="I34" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="J34">
         <v>750</v>
@@ -4003,10 +4009,10 @@
         <v>5</v>
       </c>
       <c r="N34">
+        <v>6</v>
+      </c>
+      <c r="O34">
         <v>5</v>
-      </c>
-      <c r="O34">
-        <v>4</v>
       </c>
       <c r="P34" s="4">
         <v>16</v>
@@ -4030,7 +4036,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V34">
+      <c r="V34" s="5">
         <v>0</v>
       </c>
       <c r="W34" t="s">
@@ -4048,7 +4054,7 @@
       </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="A35" s="5">
         <v>34</v>
       </c>
       <c r="B35">
@@ -4077,7 +4083,7 @@
         <v>57</v>
       </c>
       <c r="I35" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="J35">
         <v>7000</v>
@@ -4119,7 +4125,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V35">
+      <c r="V35" s="5">
         <v>1</v>
       </c>
       <c r="W35" t="s">
@@ -4137,7 +4143,7 @@
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="5">
         <v>35</v>
       </c>
       <c r="B36">
@@ -4166,7 +4172,7 @@
         <v>57</v>
       </c>
       <c r="I36" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="J36">
         <v>7000</v>
@@ -4208,7 +4214,7 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V36">
+      <c r="V36" s="5">
         <v>0</v>
       </c>
       <c r="W36" t="s">
@@ -4226,7 +4232,7 @@
       </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="A37" s="5">
         <v>36</v>
       </c>
       <c r="B37">
@@ -4249,13 +4255,13 @@
       </c>
       <c r="G37" t="str">
         <f t="shared" si="3"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="H37" t="s">
         <v>57</v>
       </c>
       <c r="I37" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="J37">
         <v>750</v>
@@ -4297,15 +4303,15 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V37">
-        <v>0</v>
+      <c r="V37" s="5">
+        <v>1</v>
       </c>
       <c r="W37" t="s">
         <v>8</v>
       </c>
       <c r="X37" t="str">
         <f t="shared" si="8"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="Y37">
         <v>0</v>
@@ -4315,7 +4321,7 @@
       </c>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="A38" s="5">
         <v>37</v>
       </c>
       <c r="B38">
@@ -4338,13 +4344,13 @@
       </c>
       <c r="G38" t="str">
         <f t="shared" si="3"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="H38" t="s">
         <v>57</v>
       </c>
       <c r="I38" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J38">
         <v>7000</v>
@@ -4386,15 +4392,15 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V38">
-        <v>0</v>
+      <c r="V38" s="5">
+        <v>1</v>
       </c>
       <c r="W38" t="s">
         <v>8</v>
       </c>
       <c r="X38" t="str">
         <f t="shared" si="8"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="Y38">
         <v>1</v>
@@ -4404,7 +4410,7 @@
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="A39" s="5">
         <v>38</v>
       </c>
       <c r="B39">
@@ -4427,13 +4433,13 @@
       </c>
       <c r="G39" t="str">
         <f t="shared" si="3"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="H39" t="s">
         <v>57</v>
       </c>
       <c r="I39" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="J39">
         <v>7000</v>
@@ -4475,15 +4481,15 @@
         <f t="shared" si="7"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V39">
-        <v>1</v>
+      <c r="V39" s="5">
+        <v>0</v>
       </c>
       <c r="W39" t="s">
         <v>8</v>
       </c>
       <c r="X39" t="str">
         <f t="shared" si="8"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="Y39">
         <v>1</v>
@@ -4493,7 +4499,7 @@
       </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="A40" s="5">
         <v>39</v>
       </c>
       <c r="B40">
@@ -4522,7 +4528,7 @@
         <v>57</v>
       </c>
       <c r="I40" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="J40">
         <v>750</v>
@@ -4564,7 +4570,7 @@
         <f t="shared" ref="U40:U71" si="16">CONCATENATE("images/choice_trial_",Q40,".png")</f>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V40">
+      <c r="V40" s="5">
         <v>1</v>
       </c>
       <c r="W40" t="s">
@@ -4582,7 +4588,7 @@
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="A41" s="5">
         <v>40</v>
       </c>
       <c r="B41">
@@ -4611,7 +4617,7 @@
         <v>57</v>
       </c>
       <c r="I41" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="J41">
         <v>750</v>
@@ -4653,7 +4659,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V41">
+      <c r="V41" s="5">
         <v>1</v>
       </c>
       <c r="W41" t="s">
@@ -4671,7 +4677,7 @@
       </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="A42" s="5">
         <v>41</v>
       </c>
       <c r="B42">
@@ -4700,7 +4706,7 @@
         <v>57</v>
       </c>
       <c r="I42" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J42">
         <v>7000</v>
@@ -4742,7 +4748,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V42">
+      <c r="V42" s="5">
         <v>1</v>
       </c>
       <c r="W42" t="s">
@@ -4760,7 +4766,7 @@
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="A43" s="5">
         <v>42</v>
       </c>
       <c r="B43">
@@ -4789,7 +4795,7 @@
         <v>57</v>
       </c>
       <c r="I43" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="J43">
         <v>750</v>
@@ -4831,7 +4837,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V43">
+      <c r="V43" s="5">
         <v>1</v>
       </c>
       <c r="W43" t="s">
@@ -4849,7 +4855,7 @@
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A44">
+      <c r="A44" s="5">
         <v>43</v>
       </c>
       <c r="B44">
@@ -4878,7 +4884,7 @@
         <v>57</v>
       </c>
       <c r="I44" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J44">
         <v>7000</v>
@@ -4920,7 +4926,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V44">
+      <c r="V44" s="5">
         <v>1</v>
       </c>
       <c r="W44" t="s">
@@ -4938,7 +4944,7 @@
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A45">
+      <c r="A45" s="5">
         <v>44</v>
       </c>
       <c r="B45">
@@ -4967,7 +4973,7 @@
         <v>57</v>
       </c>
       <c r="I45" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="J45">
         <v>750</v>
@@ -5009,7 +5015,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V45">
+      <c r="V45" s="5">
         <v>0</v>
       </c>
       <c r="W45" t="s">
@@ -5027,7 +5033,7 @@
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A46">
+      <c r="A46" s="5">
         <v>45</v>
       </c>
       <c r="B46">
@@ -5056,7 +5062,7 @@
         <v>57</v>
       </c>
       <c r="I46" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="J46">
         <v>750</v>
@@ -5098,7 +5104,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V46">
+      <c r="V46" s="5">
         <v>1</v>
       </c>
       <c r="W46" t="s">
@@ -5116,14 +5122,14 @@
       </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A47">
+      <c r="A47" s="5">
         <v>46</v>
       </c>
       <c r="B47">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="9"/>
@@ -5139,19 +5145,19 @@
       </c>
       <c r="G47" t="str">
         <f t="shared" si="12"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="H47" t="s">
         <v>57</v>
       </c>
       <c r="I47" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="J47">
         <v>7000</v>
       </c>
       <c r="K47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L47">
         <v>1</v>
@@ -5160,10 +5166,10 @@
         <v>7</v>
       </c>
       <c r="N47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P47" s="4">
         <v>14</v>
@@ -5187,15 +5193,15 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V47">
-        <v>0</v>
+      <c r="V47" s="5">
+        <v>1</v>
       </c>
       <c r="W47" t="s">
         <v>8</v>
       </c>
       <c r="X47" t="str">
         <f t="shared" si="17"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="Y47">
         <v>1</v>
@@ -5205,14 +5211,14 @@
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A48">
+      <c r="A48" s="5">
         <v>47</v>
       </c>
       <c r="B48">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="9"/>
@@ -5228,19 +5234,19 @@
       </c>
       <c r="G48" t="str">
         <f t="shared" si="12"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="H48" t="s">
         <v>57</v>
       </c>
       <c r="I48" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="J48">
         <v>7000</v>
       </c>
       <c r="K48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L48">
         <v>1</v>
@@ -5249,10 +5255,10 @@
         <v>7</v>
       </c>
       <c r="N48">
+        <v>4</v>
+      </c>
+      <c r="O48">
         <v>3</v>
-      </c>
-      <c r="O48">
-        <v>2</v>
       </c>
       <c r="P48" s="4">
         <v>14</v>
@@ -5276,15 +5282,15 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V48">
-        <v>1</v>
+      <c r="V48" s="5">
+        <v>0</v>
       </c>
       <c r="W48" t="s">
         <v>8</v>
       </c>
       <c r="X48" t="str">
         <f t="shared" si="17"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="Y48">
         <v>1</v>
@@ -5294,7 +5300,7 @@
       </c>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A49">
+      <c r="A49" s="5">
         <v>48</v>
       </c>
       <c r="B49">
@@ -5323,7 +5329,7 @@
         <v>57</v>
       </c>
       <c r="I49" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="J49">
         <v>750</v>
@@ -5365,7 +5371,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V49">
+      <c r="V49" s="5">
         <v>1</v>
       </c>
       <c r="W49" t="s">
@@ -5383,7 +5389,7 @@
       </c>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A50">
+      <c r="A50" s="5">
         <v>49</v>
       </c>
       <c r="B50">
@@ -5412,7 +5418,7 @@
         <v>57</v>
       </c>
       <c r="I50" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="J50">
         <v>750</v>
@@ -5454,7 +5460,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V50">
+      <c r="V50" s="5">
         <v>1</v>
       </c>
       <c r="W50" t="s">
@@ -5472,14 +5478,14 @@
       </c>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A51">
+      <c r="A51" s="5">
         <v>50</v>
       </c>
       <c r="B51">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C51" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="9"/>
@@ -5501,7 +5507,7 @@
         <v>57</v>
       </c>
       <c r="I51" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J51">
         <v>7000</v>
@@ -5516,10 +5522,10 @@
         <v>8</v>
       </c>
       <c r="N51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P51" s="4">
         <v>13</v>
@@ -5543,7 +5549,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V51">
+      <c r="V51" s="5">
         <v>1</v>
       </c>
       <c r="W51" t="s">
@@ -5557,18 +5563,18 @@
         <v>1</v>
       </c>
       <c r="Z51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A52">
+      <c r="A52" s="5">
         <v>51</v>
       </c>
       <c r="B52">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="9"/>
@@ -5590,7 +5596,7 @@
         <v>57</v>
       </c>
       <c r="I52" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="J52">
         <v>7000</v>
@@ -5605,10 +5611,10 @@
         <v>8</v>
       </c>
       <c r="N52">
+        <v>4</v>
+      </c>
+      <c r="O52">
         <v>3</v>
-      </c>
-      <c r="O52">
-        <v>2</v>
       </c>
       <c r="P52" s="4">
         <v>13</v>
@@ -5632,7 +5638,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V52">
+      <c r="V52" s="5">
         <v>1</v>
       </c>
       <c r="W52" t="s">
@@ -5646,11 +5652,11 @@
         <v>1</v>
       </c>
       <c r="Z52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A53">
+      <c r="A53" s="5">
         <v>52</v>
       </c>
       <c r="B53">
@@ -5679,7 +5685,7 @@
         <v>57</v>
       </c>
       <c r="I53" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="J53">
         <v>750</v>
@@ -5721,7 +5727,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V53">
+      <c r="V53" s="5">
         <v>1</v>
       </c>
       <c r="W53" t="s">
@@ -5739,7 +5745,7 @@
       </c>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A54">
+      <c r="A54" s="5">
         <v>53</v>
       </c>
       <c r="B54">
@@ -5768,7 +5774,7 @@
         <v>57</v>
       </c>
       <c r="I54" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="J54">
         <v>7000</v>
@@ -5810,7 +5816,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V54">
+      <c r="V54" s="5">
         <v>0</v>
       </c>
       <c r="W54" t="s">
@@ -5828,7 +5834,7 @@
       </c>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A55">
+      <c r="A55" s="5">
         <v>54</v>
       </c>
       <c r="B55">
@@ -5857,7 +5863,7 @@
         <v>57</v>
       </c>
       <c r="I55" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="J55">
         <v>750</v>
@@ -5899,7 +5905,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V55">
+      <c r="V55" s="5">
         <v>1</v>
       </c>
       <c r="W55" t="s">
@@ -5917,7 +5923,7 @@
       </c>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A56">
+      <c r="A56" s="5">
         <v>55</v>
       </c>
       <c r="B56">
@@ -5946,7 +5952,7 @@
         <v>57</v>
       </c>
       <c r="I56" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="J56">
         <v>7000</v>
@@ -5988,7 +5994,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V56">
+      <c r="V56" s="5">
         <v>1</v>
       </c>
       <c r="W56" t="s">
@@ -6006,7 +6012,7 @@
       </c>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A57">
+      <c r="A57" s="5">
         <v>56</v>
       </c>
       <c r="B57">
@@ -6035,7 +6041,7 @@
         <v>57</v>
       </c>
       <c r="I57" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="J57">
         <v>750</v>
@@ -6077,7 +6083,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V57">
+      <c r="V57" s="5">
         <v>0</v>
       </c>
       <c r="W57" t="s">
@@ -6095,7 +6101,7 @@
       </c>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A58">
+      <c r="A58" s="5">
         <v>57</v>
       </c>
       <c r="B58">
@@ -6124,7 +6130,7 @@
         <v>57</v>
       </c>
       <c r="I58" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J58">
         <v>7000</v>
@@ -6166,7 +6172,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V58">
+      <c r="V58" s="5">
         <v>1</v>
       </c>
       <c r="W58" t="s">
@@ -6184,7 +6190,7 @@
       </c>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A59">
+      <c r="A59" s="5">
         <v>58</v>
       </c>
       <c r="B59">
@@ -6213,7 +6219,7 @@
         <v>57</v>
       </c>
       <c r="I59" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="J59">
         <v>750</v>
@@ -6255,7 +6261,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V59">
+      <c r="V59" s="5">
         <v>1</v>
       </c>
       <c r="W59" t="s">
@@ -6273,7 +6279,7 @@
       </c>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A60">
+      <c r="A60" s="5">
         <v>59</v>
       </c>
       <c r="B60">
@@ -6302,7 +6308,7 @@
         <v>57</v>
       </c>
       <c r="I60" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="J60">
         <v>750</v>
@@ -6344,7 +6350,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V60">
+      <c r="V60" s="5">
         <v>1</v>
       </c>
       <c r="W60" t="s">
@@ -6362,7 +6368,7 @@
       </c>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A61">
+      <c r="A61" s="5">
         <v>60</v>
       </c>
       <c r="B61">
@@ -6391,7 +6397,7 @@
         <v>57</v>
       </c>
       <c r="I61" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J61">
         <v>7000</v>
@@ -6433,7 +6439,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V61">
+      <c r="V61" s="5">
         <v>1</v>
       </c>
       <c r="W61" t="s">
@@ -6451,7 +6457,7 @@
       </c>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A62">
+      <c r="A62" s="5">
         <v>61</v>
       </c>
       <c r="B62">
@@ -6480,7 +6486,7 @@
         <v>57</v>
       </c>
       <c r="I62" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="J62">
         <v>7000</v>
@@ -6522,7 +6528,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V62">
+      <c r="V62" s="5">
         <v>1</v>
       </c>
       <c r="W62" t="s">
@@ -6540,7 +6546,7 @@
       </c>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A63">
+      <c r="A63" s="5">
         <v>62</v>
       </c>
       <c r="B63">
@@ -6569,7 +6575,7 @@
         <v>57</v>
       </c>
       <c r="I63" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="J63">
         <v>750</v>
@@ -6611,7 +6617,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V63">
+      <c r="V63" s="5">
         <v>1</v>
       </c>
       <c r="W63" t="s">
@@ -6629,7 +6635,7 @@
       </c>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A64">
+      <c r="A64" s="5">
         <v>63</v>
       </c>
       <c r="B64">
@@ -6658,7 +6664,7 @@
         <v>57</v>
       </c>
       <c r="I64" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="J64">
         <v>750</v>
@@ -6700,7 +6706,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V64">
+      <c r="V64" s="5">
         <v>1</v>
       </c>
       <c r="W64" t="s">
@@ -6718,7 +6724,7 @@
       </c>
     </row>
     <row r="65" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A65">
+      <c r="A65" s="5">
         <v>64</v>
       </c>
       <c r="B65">
@@ -6747,7 +6753,7 @@
         <v>57</v>
       </c>
       <c r="I65" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J65">
         <v>7000</v>
@@ -6789,7 +6795,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V65">
+      <c r="V65" s="5">
         <v>1</v>
       </c>
       <c r="W65" t="s">
@@ -6807,7 +6813,7 @@
       </c>
     </row>
     <row r="66" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A66">
+      <c r="A66" s="5">
         <v>65</v>
       </c>
       <c r="B66">
@@ -6836,7 +6842,7 @@
         <v>57</v>
       </c>
       <c r="I66" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="J66">
         <v>750</v>
@@ -6878,7 +6884,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V66">
+      <c r="V66" s="5">
         <v>1</v>
       </c>
       <c r="W66" t="s">
@@ -6896,7 +6902,7 @@
       </c>
     </row>
     <row r="67" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A67">
+      <c r="A67" s="5">
         <v>66</v>
       </c>
       <c r="B67">
@@ -6925,7 +6931,7 @@
         <v>57</v>
       </c>
       <c r="I67" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J67">
         <v>7000</v>
@@ -6967,7 +6973,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V67">
+      <c r="V67" s="5">
         <v>1</v>
       </c>
       <c r="W67" t="s">
@@ -6985,26 +6991,26 @@
       </c>
     </row>
     <row r="68" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A68">
+      <c r="A68" s="5">
         <v>67</v>
       </c>
       <c r="B68">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="C68" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="9"/>
-        <v>images/choice_trial_16.png</v>
+        <v>images/choice_trial_3.png</v>
       </c>
       <c r="E68" t="str">
         <f t="shared" si="10"/>
-        <v>images/choice_trial_3.png</v>
+        <v>images/choice_trial_16.png</v>
       </c>
       <c r="F68" t="str">
         <f t="shared" si="11"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" si="12"/>
@@ -7014,25 +7020,25 @@
         <v>57</v>
       </c>
       <c r="I68" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="J68">
-        <v>7000</v>
+        <v>750</v>
       </c>
       <c r="K68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M68">
         <v>11</v>
       </c>
       <c r="N68">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O68">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P68" s="4">
         <v>16</v>
@@ -7042,11 +7048,11 @@
       </c>
       <c r="R68">
         <f t="shared" si="13"/>
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="S68">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="T68" t="str">
         <f t="shared" si="15"/>
@@ -7056,44 +7062,44 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V68">
-        <v>1</v>
+      <c r="V68" s="5">
+        <v>0</v>
       </c>
       <c r="W68" t="s">
         <v>8</v>
       </c>
       <c r="X68" t="str">
         <f t="shared" si="17"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="Y68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z68">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A69">
+      <c r="A69" s="5">
         <v>68</v>
       </c>
       <c r="B69">
-        <v>119</v>
+        <v>47</v>
       </c>
       <c r="C69" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="9"/>
-        <v>images/choice_trial_3.png</v>
+        <v>images/choice_trial_16.png</v>
       </c>
       <c r="E69" t="str">
         <f t="shared" si="10"/>
-        <v>images/choice_trial_16.png</v>
+        <v>images/choice_trial_3.png</v>
       </c>
       <c r="F69" t="str">
         <f t="shared" si="11"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="12"/>
@@ -7103,25 +7109,25 @@
         <v>57</v>
       </c>
       <c r="I69" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="J69">
-        <v>750</v>
+        <v>7000</v>
       </c>
       <c r="K69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M69">
         <v>11</v>
       </c>
       <c r="N69">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O69">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P69" s="4">
         <v>16</v>
@@ -7131,11 +7137,11 @@
       </c>
       <c r="R69">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="S69">
         <f t="shared" si="14"/>
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="T69" t="str">
         <f t="shared" si="15"/>
@@ -7145,25 +7151,25 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V69">
-        <v>0</v>
+      <c r="V69" s="5">
+        <v>1</v>
       </c>
       <c r="W69" t="s">
         <v>8</v>
       </c>
       <c r="X69" t="str">
         <f t="shared" si="17"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="Y69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z69">
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A70">
+      <c r="A70" s="5">
         <v>69</v>
       </c>
       <c r="B70">
@@ -7192,7 +7198,7 @@
         <v>57</v>
       </c>
       <c r="I70" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J70">
         <v>7000</v>
@@ -7234,7 +7240,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V70">
+      <c r="V70" s="5">
         <v>1</v>
       </c>
       <c r="W70" t="s">
@@ -7253,7 +7259,7 @@
       <c r="AB70" s="5"/>
     </row>
     <row r="71" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A71">
+      <c r="A71" s="5">
         <v>70</v>
       </c>
       <c r="B71">
@@ -7282,7 +7288,7 @@
         <v>57</v>
       </c>
       <c r="I71" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="J71">
         <v>750</v>
@@ -7324,7 +7330,7 @@
         <f t="shared" si="16"/>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V71">
+      <c r="V71" s="5">
         <v>1</v>
       </c>
       <c r="W71" t="s">
@@ -7342,7 +7348,7 @@
       </c>
     </row>
     <row r="72" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A72">
+      <c r="A72" s="5">
         <v>71</v>
       </c>
       <c r="B72">
@@ -7371,7 +7377,7 @@
         <v>57</v>
       </c>
       <c r="I72" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="J72">
         <v>7000</v>
@@ -7413,7 +7419,7 @@
         <f t="shared" ref="U72:U103" si="25">CONCATENATE("images/choice_trial_",Q72,".png")</f>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V72">
+      <c r="V72" s="5">
         <v>1</v>
       </c>
       <c r="W72" t="s">
@@ -7431,7 +7437,7 @@
       </c>
     </row>
     <row r="73" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A73">
+      <c r="A73" s="5">
         <v>72</v>
       </c>
       <c r="B73">
@@ -7460,7 +7466,7 @@
         <v>57</v>
       </c>
       <c r="I73" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="J73">
         <v>750</v>
@@ -7502,7 +7508,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V73">
+      <c r="V73" s="5">
         <v>1</v>
       </c>
       <c r="W73" t="s">
@@ -7520,54 +7526,54 @@
       </c>
     </row>
     <row r="74" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A74">
+      <c r="A74" s="5">
         <v>73</v>
       </c>
       <c r="B74">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="C74" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="18"/>
-        <v>images/choice_trial_12.png</v>
+        <v>images/choice_trial_6.png</v>
       </c>
       <c r="E74" t="str">
         <f t="shared" si="19"/>
-        <v>images/choice_trial_6.png</v>
+        <v>images/choice_trial_12.png</v>
       </c>
       <c r="F74" t="str">
         <f t="shared" si="20"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="21"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="H74" t="s">
         <v>57</v>
       </c>
       <c r="I74" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="J74">
-        <v>7000</v>
+        <v>750</v>
       </c>
       <c r="K74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M74">
         <v>12</v>
       </c>
       <c r="N74">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O74">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P74" s="4">
         <v>6</v>
@@ -7577,11 +7583,11 @@
       </c>
       <c r="R74">
         <f t="shared" si="22"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="S74">
         <f t="shared" si="23"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="T74" t="str">
         <f t="shared" si="24"/>
@@ -7591,7 +7597,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V74">
+      <c r="V74" s="5">
         <v>1</v>
       </c>
       <c r="W74" t="s">
@@ -7602,61 +7608,61 @@
         <v>f</v>
       </c>
       <c r="Y74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z74">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A75">
+      <c r="A75" s="5">
         <v>74</v>
       </c>
       <c r="B75">
-        <v>120</v>
+        <v>48</v>
       </c>
       <c r="C75" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="18"/>
-        <v>images/choice_trial_6.png</v>
+        <v>images/choice_trial_12.png</v>
       </c>
       <c r="E75" t="str">
         <f t="shared" si="19"/>
-        <v>images/choice_trial_12.png</v>
+        <v>images/choice_trial_6.png</v>
       </c>
       <c r="F75" t="str">
         <f t="shared" si="20"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" si="21"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="H75" t="s">
         <v>57</v>
       </c>
       <c r="I75" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="J75">
-        <v>750</v>
+        <v>7000</v>
       </c>
       <c r="K75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M75">
         <v>12</v>
       </c>
       <c r="N75">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O75">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P75" s="4">
         <v>6</v>
@@ -7666,11 +7672,11 @@
       </c>
       <c r="R75">
         <f t="shared" si="22"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="S75">
         <f t="shared" si="23"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="T75" t="str">
         <f t="shared" si="24"/>
@@ -7680,7 +7686,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V75">
+      <c r="V75" s="5">
         <v>1</v>
       </c>
       <c r="W75" t="s">
@@ -7691,14 +7697,14 @@
         <v>f</v>
       </c>
       <c r="Y75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z75">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A76">
+      <c r="A76" s="5">
         <v>75</v>
       </c>
       <c r="B76">
@@ -7727,7 +7733,7 @@
         <v>57</v>
       </c>
       <c r="I76" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J76">
         <v>7000</v>
@@ -7769,7 +7775,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V76">
+      <c r="V76" s="5">
         <v>1</v>
       </c>
       <c r="W76" t="s">
@@ -7787,7 +7793,7 @@
       </c>
     </row>
     <row r="77" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A77">
+      <c r="A77" s="5">
         <v>76</v>
       </c>
       <c r="B77">
@@ -7816,7 +7822,7 @@
         <v>57</v>
       </c>
       <c r="I77" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="J77">
         <v>750</v>
@@ -7858,7 +7864,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V77">
+      <c r="V77" s="5">
         <v>1</v>
       </c>
       <c r="W77" t="s">
@@ -7877,26 +7883,26 @@
       <c r="AB77" s="5"/>
     </row>
     <row r="78" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A78">
+      <c r="A78" s="5">
         <v>77</v>
       </c>
       <c r="B78">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="C78" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="18"/>
-        <v>images/choice_trial_6.png</v>
+        <v>images/choice_trial_12.png</v>
       </c>
       <c r="E78" t="str">
         <f t="shared" si="19"/>
-        <v>images/choice_trial_12.png</v>
+        <v>images/choice_trial_6.png</v>
       </c>
       <c r="F78" t="str">
         <f t="shared" si="20"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="G78" t="str">
         <f t="shared" si="21"/>
@@ -7906,25 +7912,25 @@
         <v>57</v>
       </c>
       <c r="I78" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="J78">
-        <v>7000</v>
+        <v>750</v>
       </c>
       <c r="K78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M78">
         <v>12</v>
       </c>
       <c r="N78">
+        <v>5</v>
+      </c>
+      <c r="O78">
         <v>4</v>
-      </c>
-      <c r="O78">
-        <v>3</v>
       </c>
       <c r="P78" s="4">
         <v>6</v>
@@ -7934,11 +7940,11 @@
       </c>
       <c r="R78">
         <f t="shared" si="22"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="S78">
         <f t="shared" si="23"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="T78" t="str">
         <f t="shared" si="24"/>
@@ -7948,44 +7954,44 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V78">
-        <v>0</v>
+      <c r="V78" s="5">
+        <v>1</v>
       </c>
       <c r="W78" t="s">
         <v>8</v>
       </c>
       <c r="X78" t="str">
         <f t="shared" si="26"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="Y78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z78">
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A79">
+      <c r="A79" s="5">
         <v>78</v>
       </c>
       <c r="B79">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C79" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="18"/>
-        <v>images/choice_trial_12.png</v>
+        <v>images/choice_trial_6.png</v>
       </c>
       <c r="E79" t="str">
         <f t="shared" si="19"/>
-        <v>images/choice_trial_6.png</v>
+        <v>images/choice_trial_12.png</v>
       </c>
       <c r="F79" t="str">
         <f t="shared" si="20"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="G79" t="str">
         <f t="shared" si="21"/>
@@ -7995,25 +8001,25 @@
         <v>57</v>
       </c>
       <c r="I79" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="J79">
-        <v>750</v>
+        <v>7000</v>
       </c>
       <c r="K79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M79">
         <v>12</v>
       </c>
       <c r="N79">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O79">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P79" s="4">
         <v>6</v>
@@ -8023,11 +8029,11 @@
       </c>
       <c r="R79">
         <f t="shared" si="22"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="S79">
         <f t="shared" si="23"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="T79" t="str">
         <f t="shared" si="24"/>
@@ -8037,25 +8043,25 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V79">
-        <v>1</v>
+      <c r="V79" s="5">
+        <v>0</v>
       </c>
       <c r="W79" t="s">
         <v>8</v>
       </c>
       <c r="X79" t="str">
         <f t="shared" si="26"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="Y79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z79">
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A80">
+      <c r="A80" s="5">
         <v>79</v>
       </c>
       <c r="B80">
@@ -8084,7 +8090,7 @@
         <v>57</v>
       </c>
       <c r="I80" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="J80">
         <v>750</v>
@@ -8126,7 +8132,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V80">
+      <c r="V80" s="5">
         <v>1</v>
       </c>
       <c r="W80" t="s">
@@ -8144,7 +8150,7 @@
       </c>
     </row>
     <row r="81" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A81">
+      <c r="A81" s="5">
         <v>80</v>
       </c>
       <c r="B81">
@@ -8173,7 +8179,7 @@
         <v>57</v>
       </c>
       <c r="I81" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="J81">
         <v>750</v>
@@ -8215,7 +8221,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V81">
+      <c r="V81" s="5">
         <v>1</v>
       </c>
       <c r="W81" t="s">
@@ -8233,54 +8239,54 @@
       </c>
     </row>
     <row r="82" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A82">
+      <c r="A82" s="5">
         <v>81</v>
       </c>
       <c r="B82">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="C82" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="18"/>
-        <v>images/choice_trial_8.png</v>
+        <v>images/choice_trial_14.png</v>
       </c>
       <c r="E82" t="str">
         <f t="shared" si="19"/>
-        <v>images/choice_trial_14.png</v>
+        <v>images/choice_trial_8.png</v>
       </c>
       <c r="F82" t="str">
         <f t="shared" si="20"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="G82" t="str">
         <f t="shared" si="21"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="H82" t="s">
         <v>57</v>
       </c>
       <c r="I82" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J82">
-        <v>7000</v>
+        <v>750</v>
       </c>
       <c r="K82">
         <v>0</v>
       </c>
       <c r="L82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M82">
         <v>13</v>
       </c>
       <c r="N82">
+        <v>5</v>
+      </c>
+      <c r="O82">
         <v>4</v>
-      </c>
-      <c r="O82">
-        <v>3</v>
       </c>
       <c r="P82" s="4">
         <v>14</v>
@@ -8290,11 +8296,11 @@
       </c>
       <c r="R82">
         <f t="shared" si="22"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="S82">
         <f t="shared" si="23"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="T82" t="str">
         <f t="shared" si="24"/>
@@ -8304,7 +8310,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V82">
+      <c r="V82" s="5">
         <v>1</v>
       </c>
       <c r="W82" t="s">
@@ -8315,61 +8321,61 @@
         <v>f</v>
       </c>
       <c r="Y82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z82">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A83">
+      <c r="A83" s="5">
         <v>82</v>
       </c>
       <c r="B83">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C83" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="18"/>
-        <v>images/choice_trial_14.png</v>
+        <v>images/choice_trial_8.png</v>
       </c>
       <c r="E83" t="str">
         <f t="shared" si="19"/>
-        <v>images/choice_trial_8.png</v>
+        <v>images/choice_trial_14.png</v>
       </c>
       <c r="F83" t="str">
         <f t="shared" si="20"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="G83" t="str">
         <f t="shared" si="21"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="H83" t="s">
         <v>57</v>
       </c>
       <c r="I83" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="J83">
-        <v>750</v>
+        <v>7000</v>
       </c>
       <c r="K83">
         <v>0</v>
       </c>
       <c r="L83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M83">
         <v>13</v>
       </c>
       <c r="N83">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O83">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P83" s="4">
         <v>14</v>
@@ -8379,11 +8385,11 @@
       </c>
       <c r="R83">
         <f t="shared" si="22"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="S83">
         <f t="shared" si="23"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="T83" t="str">
         <f t="shared" si="24"/>
@@ -8393,7 +8399,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V83">
+      <c r="V83" s="5">
         <v>1</v>
       </c>
       <c r="W83" t="s">
@@ -8404,14 +8410,14 @@
         <v>f</v>
       </c>
       <c r="Y83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z83">
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A84">
+      <c r="A84" s="5">
         <v>83</v>
       </c>
       <c r="B84">
@@ -8440,7 +8446,7 @@
         <v>57</v>
       </c>
       <c r="I84" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J84">
         <v>7000</v>
@@ -8482,7 +8488,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V84">
+      <c r="V84" s="5">
         <v>1</v>
       </c>
       <c r="W84" t="s">
@@ -8500,7 +8506,7 @@
       </c>
     </row>
     <row r="85" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A85">
+      <c r="A85" s="5">
         <v>84</v>
       </c>
       <c r="B85">
@@ -8529,7 +8535,7 @@
         <v>57</v>
       </c>
       <c r="I85" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="J85">
         <v>7000</v>
@@ -8571,7 +8577,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_8.png</v>
       </c>
-      <c r="V85">
+      <c r="V85" s="5">
         <v>1</v>
       </c>
       <c r="W85" t="s">
@@ -8589,7 +8595,7 @@
       </c>
     </row>
     <row r="86" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A86">
+      <c r="A86" s="5">
         <v>85</v>
       </c>
       <c r="B86">
@@ -8618,7 +8624,7 @@
         <v>57</v>
       </c>
       <c r="I86" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="J86">
         <v>750</v>
@@ -8660,7 +8666,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V86">
+      <c r="V86" s="5">
         <v>1</v>
       </c>
       <c r="W86" t="s">
@@ -8678,7 +8684,7 @@
       </c>
     </row>
     <row r="87" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A87">
+      <c r="A87" s="5">
         <v>86</v>
       </c>
       <c r="B87">
@@ -8707,7 +8713,7 @@
         <v>57</v>
       </c>
       <c r="I87" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="J87">
         <v>750</v>
@@ -8749,7 +8755,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V87">
+      <c r="V87" s="5">
         <v>1</v>
       </c>
       <c r="W87" t="s">
@@ -8767,7 +8773,7 @@
       </c>
     </row>
     <row r="88" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A88">
+      <c r="A88" s="5">
         <v>87</v>
       </c>
       <c r="B88">
@@ -8796,7 +8802,7 @@
         <v>57</v>
       </c>
       <c r="I88" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J88">
         <v>7000</v>
@@ -8838,7 +8844,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V88">
+      <c r="V88" s="5">
         <v>0</v>
       </c>
       <c r="W88" t="s">
@@ -8857,7 +8863,7 @@
       <c r="AB88" s="5"/>
     </row>
     <row r="89" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A89">
+      <c r="A89" s="5">
         <v>88</v>
       </c>
       <c r="B89">
@@ -8886,7 +8892,7 @@
         <v>57</v>
       </c>
       <c r="I89" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J89">
         <v>7000</v>
@@ -8928,7 +8934,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V89">
+      <c r="V89" s="5">
         <v>1</v>
       </c>
       <c r="W89" t="s">
@@ -8946,7 +8952,7 @@
       </c>
     </row>
     <row r="90" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A90">
+      <c r="A90" s="5">
         <v>89</v>
       </c>
       <c r="B90">
@@ -8975,7 +8981,7 @@
         <v>57</v>
       </c>
       <c r="I90" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="J90">
         <v>750</v>
@@ -9017,7 +9023,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V90">
+      <c r="V90" s="5">
         <v>0</v>
       </c>
       <c r="W90" t="s">
@@ -9035,7 +9041,7 @@
       </c>
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A91">
+      <c r="A91" s="5">
         <v>90</v>
       </c>
       <c r="B91">
@@ -9064,7 +9070,7 @@
         <v>57</v>
       </c>
       <c r="I91" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="J91">
         <v>7000</v>
@@ -9106,7 +9112,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_10.png</v>
       </c>
-      <c r="V91">
+      <c r="V91" s="5">
         <v>0</v>
       </c>
       <c r="W91" t="s">
@@ -9124,7 +9130,7 @@
       </c>
     </row>
     <row r="92" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A92">
+      <c r="A92" s="5">
         <v>91</v>
       </c>
       <c r="B92">
@@ -9153,7 +9159,7 @@
         <v>57</v>
       </c>
       <c r="I92" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="J92">
         <v>750</v>
@@ -9195,7 +9201,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V92">
+      <c r="V92" s="5">
         <v>0</v>
       </c>
       <c r="W92" t="s">
@@ -9213,7 +9219,7 @@
       </c>
     </row>
     <row r="93" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A93">
+      <c r="A93" s="5">
         <v>92</v>
       </c>
       <c r="B93">
@@ -9242,7 +9248,7 @@
         <v>57</v>
       </c>
       <c r="I93" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J93">
         <v>7000</v>
@@ -9284,7 +9290,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V93">
+      <c r="V93" s="5">
         <v>1</v>
       </c>
       <c r="W93" t="s">
@@ -9302,7 +9308,7 @@
       </c>
     </row>
     <row r="94" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A94">
+      <c r="A94" s="5">
         <v>93</v>
       </c>
       <c r="B94">
@@ -9331,7 +9337,7 @@
         <v>57</v>
       </c>
       <c r="I94" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="J94">
         <v>750</v>
@@ -9373,7 +9379,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V94">
+      <c r="V94" s="5">
         <v>1</v>
       </c>
       <c r="W94" t="s">
@@ -9391,7 +9397,7 @@
       </c>
     </row>
     <row r="95" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A95">
+      <c r="A95" s="5">
         <v>94</v>
       </c>
       <c r="B95">
@@ -9420,7 +9426,7 @@
         <v>57</v>
       </c>
       <c r="I95" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="J95">
         <v>7000</v>
@@ -9462,7 +9468,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V95">
+      <c r="V95" s="5">
         <v>1</v>
       </c>
       <c r="W95" t="s">
@@ -9481,7 +9487,7 @@
       <c r="AB95" s="5"/>
     </row>
     <row r="96" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A96">
+      <c r="A96" s="5">
         <v>95</v>
       </c>
       <c r="B96">
@@ -9510,7 +9516,7 @@
         <v>57</v>
       </c>
       <c r="I96" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="J96">
         <v>750</v>
@@ -9552,7 +9558,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V96">
+      <c r="V96" s="5">
         <v>1</v>
       </c>
       <c r="W96" t="s">
@@ -9570,7 +9576,7 @@
       </c>
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A97">
+      <c r="A97" s="5">
         <v>96</v>
       </c>
       <c r="B97">
@@ -9599,7 +9605,7 @@
         <v>57</v>
       </c>
       <c r="I97" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="J97">
         <v>7000</v>
@@ -9641,7 +9647,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_9.png</v>
       </c>
-      <c r="V97">
+      <c r="V97" s="5">
         <v>0</v>
       </c>
       <c r="W97" t="s">
@@ -9659,7 +9665,7 @@
       </c>
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A98">
+      <c r="A98" s="5">
         <v>97</v>
       </c>
       <c r="B98">
@@ -9688,7 +9694,7 @@
         <v>57</v>
       </c>
       <c r="I98" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J98">
         <v>7000</v>
@@ -9730,7 +9736,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V98">
+      <c r="V98" s="5">
         <v>1</v>
       </c>
       <c r="W98" t="s">
@@ -9748,7 +9754,7 @@
       </c>
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A99">
+      <c r="A99" s="5">
         <v>98</v>
       </c>
       <c r="B99">
@@ -9777,7 +9783,7 @@
         <v>57</v>
       </c>
       <c r="I99" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="J99">
         <v>750</v>
@@ -9819,7 +9825,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V99">
+      <c r="V99" s="5">
         <v>0</v>
       </c>
       <c r="W99" t="s">
@@ -9837,7 +9843,7 @@
       </c>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A100">
+      <c r="A100" s="5">
         <v>99</v>
       </c>
       <c r="B100">
@@ -9866,7 +9872,7 @@
         <v>57</v>
       </c>
       <c r="I100" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="J100">
         <v>750</v>
@@ -9908,7 +9914,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V100">
+      <c r="V100" s="5">
         <v>1</v>
       </c>
       <c r="W100" t="s">
@@ -9926,7 +9932,7 @@
       </c>
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A101">
+      <c r="A101" s="5">
         <v>100</v>
       </c>
       <c r="B101">
@@ -9955,7 +9961,7 @@
         <v>57</v>
       </c>
       <c r="I101" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="J101">
         <v>750</v>
@@ -9997,7 +10003,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V101">
+      <c r="V101" s="5">
         <v>0</v>
       </c>
       <c r="W101" t="s">
@@ -10015,7 +10021,7 @@
       </c>
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A102">
+      <c r="A102" s="5">
         <v>101</v>
       </c>
       <c r="B102">
@@ -10044,7 +10050,7 @@
         <v>57</v>
       </c>
       <c r="I102" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="J102">
         <v>7000</v>
@@ -10086,7 +10092,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V102">
+      <c r="V102" s="5">
         <v>0</v>
       </c>
       <c r="W102" t="s">
@@ -10104,7 +10110,7 @@
       </c>
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A103">
+      <c r="A103" s="5">
         <v>102</v>
       </c>
       <c r="B103">
@@ -10133,7 +10139,7 @@
         <v>57</v>
       </c>
       <c r="I103" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J103">
         <v>7000</v>
@@ -10175,7 +10181,7 @@
         <f t="shared" si="25"/>
         <v>images/choice_trial_2.png</v>
       </c>
-      <c r="V103">
+      <c r="V103" s="5">
         <v>1</v>
       </c>
       <c r="W103" t="s">
@@ -10193,7 +10199,7 @@
       </c>
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A104">
+      <c r="A104" s="5">
         <v>103</v>
       </c>
       <c r="B104">
@@ -10222,7 +10228,7 @@
         <v>57</v>
       </c>
       <c r="I104" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="J104">
         <v>750</v>
@@ -10264,7 +10270,7 @@
         <f t="shared" ref="U104:U115" si="34">CONCATENATE("images/choice_trial_",Q104,".png")</f>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V104">
+      <c r="V104" s="5">
         <v>1</v>
       </c>
       <c r="W104" t="s">
@@ -10282,7 +10288,7 @@
       </c>
     </row>
     <row r="105" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A105">
+      <c r="A105" s="5">
         <v>104</v>
       </c>
       <c r="B105">
@@ -10311,7 +10317,7 @@
         <v>57</v>
       </c>
       <c r="I105" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="J105">
         <v>750</v>
@@ -10353,7 +10359,7 @@
         <f t="shared" si="34"/>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V105">
+      <c r="V105" s="5">
         <v>1</v>
       </c>
       <c r="W105" t="s">
@@ -10371,7 +10377,7 @@
       </c>
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A106">
+      <c r="A106" s="5">
         <v>105</v>
       </c>
       <c r="B106">
@@ -10400,7 +10406,7 @@
         <v>57</v>
       </c>
       <c r="I106" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J106">
         <v>7000</v>
@@ -10442,7 +10448,7 @@
         <f t="shared" si="34"/>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V106">
+      <c r="V106" s="5">
         <v>1</v>
       </c>
       <c r="W106" t="s">
@@ -10460,7 +10466,7 @@
       </c>
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A107">
+      <c r="A107" s="5">
         <v>106</v>
       </c>
       <c r="B107">
@@ -10489,7 +10495,7 @@
         <v>57</v>
       </c>
       <c r="I107" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="J107">
         <v>750</v>
@@ -10531,7 +10537,7 @@
         <f t="shared" si="34"/>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V107">
+      <c r="V107" s="5">
         <v>0</v>
       </c>
       <c r="W107" t="s">
@@ -10549,7 +10555,7 @@
       </c>
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A108">
+      <c r="A108" s="5">
         <v>107</v>
       </c>
       <c r="B108">
@@ -10578,7 +10584,7 @@
         <v>57</v>
       </c>
       <c r="I108" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J108">
         <v>7000</v>
@@ -10620,7 +10626,7 @@
         <f t="shared" si="34"/>
         <v>images/choice_trial_3.png</v>
       </c>
-      <c r="V108">
+      <c r="V108" s="5">
         <v>1</v>
       </c>
       <c r="W108" t="s">
@@ -10638,78 +10644,78 @@
       </c>
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A109">
+      <c r="A109" s="5">
         <v>108</v>
       </c>
       <c r="B109">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="C109" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D109" t="str">
         <f t="shared" si="27"/>
-        <v>images/choice_trial_16.png</v>
+        <v>images/choice_trial_12.png</v>
       </c>
       <c r="E109" t="str">
         <f t="shared" si="28"/>
-        <v>images/choice_trial_3.png</v>
+        <v>images/choice_trial_6.png</v>
       </c>
       <c r="F109" t="str">
         <f t="shared" si="29"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="G109" t="str">
         <f t="shared" si="30"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="H109" t="s">
         <v>57</v>
       </c>
       <c r="I109" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="J109">
-        <v>7000</v>
+        <v>750</v>
       </c>
       <c r="K109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M109">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N109">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O109">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P109" s="4">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="Q109" s="4">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="R109">
         <f t="shared" si="31"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="S109">
         <f t="shared" si="32"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T109" t="str">
         <f t="shared" si="33"/>
-        <v>images/choice_trial_16.png</v>
+        <v>images/choice_trial_6.png</v>
       </c>
       <c r="U109" t="str">
         <f t="shared" si="34"/>
-        <v>images/choice_trial_3.png</v>
-      </c>
-      <c r="V109">
+        <v>images/choice_trial_12.png</v>
+      </c>
+      <c r="V109" s="5">
         <v>1</v>
       </c>
       <c r="W109" t="s">
@@ -10720,85 +10726,85 @@
         <v>f</v>
       </c>
       <c r="Y109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z109">
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A110">
+      <c r="A110" s="5">
         <v>109</v>
       </c>
       <c r="B110">
-        <v>108</v>
+        <v>53</v>
       </c>
       <c r="C110" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D110" t="str">
         <f t="shared" si="27"/>
-        <v>images/choice_trial_12.png</v>
+        <v>images/choice_trial_16.png</v>
       </c>
       <c r="E110" t="str">
         <f t="shared" si="28"/>
-        <v>images/choice_trial_6.png</v>
+        <v>images/choice_trial_3.png</v>
       </c>
       <c r="F110" t="str">
         <f t="shared" si="29"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="G110" t="str">
         <f t="shared" si="30"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="H110" t="s">
         <v>57</v>
       </c>
       <c r="I110" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="J110">
-        <v>750</v>
+        <v>7000</v>
       </c>
       <c r="K110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M110">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N110">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O110">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P110" s="4">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="Q110" s="4">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="R110">
         <f t="shared" si="31"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="S110">
         <f t="shared" si="32"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="T110" t="str">
         <f t="shared" si="33"/>
-        <v>images/choice_trial_6.png</v>
+        <v>images/choice_trial_16.png</v>
       </c>
       <c r="U110" t="str">
         <f t="shared" si="34"/>
-        <v>images/choice_trial_12.png</v>
-      </c>
-      <c r="V110">
+        <v>images/choice_trial_3.png</v>
+      </c>
+      <c r="V110" s="5">
         <v>1</v>
       </c>
       <c r="W110" t="s">
@@ -10809,14 +10815,14 @@
         <v>f</v>
       </c>
       <c r="Y110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z110">
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A111">
+      <c r="A111" s="5">
         <v>110</v>
       </c>
       <c r="B111">
@@ -10845,7 +10851,7 @@
         <v>57</v>
       </c>
       <c r="I111" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="J111">
         <v>750</v>
@@ -10887,7 +10893,7 @@
         <f t="shared" si="34"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V111">
+      <c r="V111" s="5">
         <v>1</v>
       </c>
       <c r="W111" t="s">
@@ -10905,7 +10911,7 @@
       </c>
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A112">
+      <c r="A112" s="5">
         <v>111</v>
       </c>
       <c r="B112">
@@ -10934,7 +10940,7 @@
         <v>57</v>
       </c>
       <c r="I112" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J112">
         <v>7000</v>
@@ -10976,7 +10982,7 @@
         <f t="shared" si="34"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V112">
+      <c r="V112" s="5">
         <v>1</v>
       </c>
       <c r="W112" t="s">
@@ -10994,14 +11000,14 @@
       </c>
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A113">
+      <c r="A113" s="5">
         <v>112</v>
       </c>
       <c r="B113">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="C113" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D113" t="str">
         <f t="shared" si="27"/>
@@ -11017,19 +11023,19 @@
       </c>
       <c r="G113" t="str">
         <f t="shared" si="30"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="H113" t="s">
         <v>57</v>
       </c>
       <c r="I113" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="J113">
-        <v>750</v>
+        <v>7000</v>
       </c>
       <c r="K113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L113">
         <v>0</v>
@@ -11038,10 +11044,10 @@
         <v>18</v>
       </c>
       <c r="N113">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O113">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="P113" s="4">
         <v>6</v>
@@ -11065,32 +11071,32 @@
         <f t="shared" si="34"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V113">
-        <v>1</v>
+      <c r="V113" s="5">
+        <v>0</v>
       </c>
       <c r="W113" t="s">
         <v>8</v>
       </c>
       <c r="X113" t="str">
         <f t="shared" si="35"/>
-        <v>f</v>
+        <v>j</v>
       </c>
       <c r="Y113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z113">
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A114">
+      <c r="A114" s="5">
         <v>113</v>
       </c>
       <c r="B114">
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="C114" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D114" t="str">
         <f t="shared" si="27"/>
@@ -11106,19 +11112,19 @@
       </c>
       <c r="G114" t="str">
         <f t="shared" si="30"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="H114" t="s">
         <v>57</v>
       </c>
       <c r="I114" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="J114">
-        <v>7000</v>
+        <v>750</v>
       </c>
       <c r="K114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L114">
         <v>0</v>
@@ -11127,10 +11133,10 @@
         <v>18</v>
       </c>
       <c r="N114">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O114">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P114" s="4">
         <v>6</v>
@@ -11154,25 +11160,25 @@
         <f t="shared" si="34"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V114">
-        <v>0</v>
+      <c r="V114" s="5">
+        <v>1</v>
       </c>
       <c r="W114" t="s">
         <v>8</v>
       </c>
       <c r="X114" t="str">
         <f t="shared" si="35"/>
-        <v>j</v>
+        <v>f</v>
       </c>
       <c r="Y114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z114">
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A115">
+      <c r="A115" s="5">
         <v>114</v>
       </c>
       <c r="B115">
@@ -11201,7 +11207,7 @@
         <v>57</v>
       </c>
       <c r="I115" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="J115">
         <v>7000</v>
@@ -11243,7 +11249,7 @@
         <f t="shared" si="34"/>
         <v>images/choice_trial_12.png</v>
       </c>
-      <c r="V115">
+      <c r="V115" s="5">
         <v>1</v>
       </c>
       <c r="W115" t="s">

</xml_diff>